<commit_message>
column aliases and spreadsheet fixes
</commit_message>
<xml_diff>
--- a/src/server/data/empty-template.xlsx
+++ b/src/server/data/empty-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnmclaughlin/git/usdr/cares-reporter/src/server/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD83156F-1486-7046-B68B-AB35775B3EB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914309C2-D981-1741-8A0F-10717B68C037}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3980" yWindow="-20940" windowWidth="28900" windowHeight="20540" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="216">
   <si>
     <t>Agency Code</t>
   </si>
@@ -239,15 +239,6 @@
     <t xml:space="preserve">Award Date </t>
   </si>
   <si>
-    <t xml:space="preserve">Awardee Primary Place of Performance Address Line 1 </t>
-  </si>
-  <si>
-    <t>Awardee Primary Place of Performance Address Line 2</t>
-  </si>
-  <si>
-    <t>Awardee Primary Place of Performance Address Line 3</t>
-  </si>
-  <si>
     <t>Primary Place of Performance Country Name</t>
   </si>
   <si>
@@ -371,9 +362,6 @@
     <t>RI Other Expenditure Categories</t>
   </si>
   <si>
-    <t>Is Awardee Complying with Terms and Conditions of the Grant?</t>
-  </si>
-  <si>
     <t>Dropdown Options</t>
   </si>
   <si>
@@ -705,6 +693,9 @@
   </si>
   <si>
     <t>Sum of Expenses</t>
+  </si>
+  <si>
+    <t>Compliance</t>
   </si>
 </sst>
 </file>
@@ -1293,10 +1284,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4336,13 +4327,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5352,8 +5343,8 @@
   </sheetPr>
   <dimension ref="A1:AA61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5370,49 +5361,49 @@
   <sheetData>
     <row r="1" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="E1" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="G1" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="I1" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="G1" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="H1" s="14" t="s">
+      <c r="L1" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="M1" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="N1" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="O1" s="14" t="s">
         <v>99</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="M1" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="N1" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="O1" s="14" t="s">
-        <v>102</v>
       </c>
       <c r="P1" s="14"/>
       <c r="Q1" s="14"/>
@@ -5429,7 +5420,7 @@
     </row>
     <row r="2" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>7</v>
@@ -5441,37 +5432,37 @@
         <v>16</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F2" s="16" t="s">
         <v>21</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I2" s="16" t="s">
         <v>60</v>
       </c>
       <c r="J2" s="16" t="s">
-        <v>107</v>
+        <v>215</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="M2" s="16" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="N2" s="16" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="O2" s="16" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="P2" s="14"/>
       <c r="Q2" s="14"/>
@@ -5488,473 +5479,473 @@
     </row>
     <row r="3" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="F3" s="17" t="s">
         <v>108</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>112</v>
       </c>
       <c r="G3" s="17">
         <v>1</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I3" s="17" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="J3" s="17" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="K3" s="17" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="L3" s="17" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="N3" s="17" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="O3" s="17" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="F4" s="17" t="s">
         <v>116</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>120</v>
       </c>
       <c r="G4" s="17">
         <v>2</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="K4" s="17" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="M4" s="17" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="N4" s="17" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="O4" s="17" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="F5" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C5" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>129</v>
-      </c>
       <c r="G5" s="19" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M5" s="17" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="M6" s="17" t="s">
         <v>130</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="M6" s="17" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="17" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="M7" s="17" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="18" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E8" s="20"/>
     </row>
     <row r="9" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="18" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="17" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="18" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="18" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C13" s="18" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C14" s="17" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C15" s="17" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C16" s="17" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17" s="17" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C18" s="17" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C19" s="17" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C20" s="17" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C21" s="17" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C22" s="18" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C23" s="18" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C24" s="18" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="25" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C25" s="17" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C26" s="17" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="27" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D27" s="17" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="28" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C28" s="18"/>
       <c r="D28" s="17" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="29" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D29" s="17" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="30" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D30" s="17" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="31" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D31" s="17" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="32" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D32" s="17" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="33" spans="4:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D33" s="17" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="34" spans="4:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D34" s="17" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="35" spans="4:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D35" s="17" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="36" spans="4:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D36" s="17" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="37" spans="4:4" ht="14" x14ac:dyDescent="0.2">
       <c r="D37" s="17" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="38" spans="4:4" ht="14" x14ac:dyDescent="0.2">
       <c r="D38" s="17" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="39" spans="4:4" ht="14" x14ac:dyDescent="0.2">
       <c r="D39" s="17" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="40" spans="4:4" ht="14" x14ac:dyDescent="0.2">
       <c r="D40" s="17" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="41" spans="4:4" ht="14" x14ac:dyDescent="0.2">
       <c r="D41" s="17" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="42" spans="4:4" ht="14" x14ac:dyDescent="0.2">
       <c r="D42" s="17" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="43" spans="4:4" ht="14" x14ac:dyDescent="0.2">
       <c r="D43" s="17" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="44" spans="4:4" ht="14" x14ac:dyDescent="0.2">
       <c r="D44" s="17" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="45" spans="4:4" ht="14" x14ac:dyDescent="0.2">
       <c r="D45" s="17" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="46" spans="4:4" ht="14" x14ac:dyDescent="0.2">
       <c r="D46" s="17" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="47" spans="4:4" ht="14" x14ac:dyDescent="0.2">
       <c r="D47" s="17" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="48" spans="4:4" ht="14" x14ac:dyDescent="0.2">
       <c r="D48" s="17" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="49" spans="4:4" ht="14" x14ac:dyDescent="0.2">
       <c r="D49" s="17" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="50" spans="4:4" ht="14" x14ac:dyDescent="0.2">
       <c r="D50" s="17" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="51" spans="4:4" ht="14" x14ac:dyDescent="0.2">
       <c r="D51" s="17" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="52" spans="4:4" ht="14" x14ac:dyDescent="0.2">
       <c r="D52" s="17" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="53" spans="4:4" ht="14" x14ac:dyDescent="0.2">
       <c r="D53" s="17" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="54" spans="4:4" ht="14" x14ac:dyDescent="0.2">
       <c r="D54" s="17" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="55" spans="4:4" ht="14" x14ac:dyDescent="0.2">
       <c r="D55" s="17" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="56" spans="4:4" ht="14" x14ac:dyDescent="0.2">
       <c r="D56" s="17" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="57" spans="4:4" ht="14" x14ac:dyDescent="0.2">
       <c r="D57" s="17" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="58" spans="4:4" ht="14" x14ac:dyDescent="0.2">
       <c r="D58" s="17" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="59" spans="4:4" ht="14" x14ac:dyDescent="0.2">
       <c r="D59" s="17" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="60" spans="4:4" ht="14" x14ac:dyDescent="0.2">
       <c r="D60" s="17" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="61" spans="4:4" ht="14" x14ac:dyDescent="0.2">
       <c r="D61" s="17" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -6209,10 +6200,10 @@
         <v>35</v>
       </c>
       <c r="B1" s="42" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D1" s="42" t="s">
         <v>20</v>
@@ -6329,7 +6320,7 @@
         <v>57</v>
       </c>
       <c r="AP1" s="37" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -6348,7 +6339,7 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AS1" sqref="AS1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6391,10 +6382,10 @@
         <v>35</v>
       </c>
       <c r="B1" s="42" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D1" s="38" t="s">
         <v>59</v>
@@ -6414,14 +6405,14 @@
       <c r="I1" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="K1" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="L1" s="29" t="s">
-        <v>65</v>
+      <c r="J1" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="24" t="s">
+        <v>28</v>
       </c>
       <c r="M1" s="29" t="s">
         <v>29</v>
@@ -6433,19 +6424,19 @@
         <v>31</v>
       </c>
       <c r="P1" s="29" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Q1" s="29" t="s">
         <v>33</v>
       </c>
       <c r="R1" s="29" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="S1" s="29" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="T1" s="29" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="U1" s="53" t="s">
         <v>36</v>
@@ -6517,7 +6508,7 @@
         <v>57</v>
       </c>
       <c r="AR1" s="54" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -6534,9 +6525,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AO5"/>
   <sheetViews>
-    <sheetView topLeftCell="X1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="M1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AP1" sqref="AP1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="AL1" sqref="AL1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6574,25 +6565,25 @@
         <v>35</v>
       </c>
       <c r="B1" s="42" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D1" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>209</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="E1" s="49" t="s">
-        <v>71</v>
-      </c>
-      <c r="F1" s="40" t="s">
-        <v>213</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>27</v>
@@ -6601,22 +6592,22 @@
         <v>28</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>31</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>33</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>36</v>
@@ -6625,13 +6616,13 @@
         <v>35</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="V1" s="4" t="s">
         <v>40</v>
@@ -6691,7 +6682,7 @@
         <v>57</v>
       </c>
       <c r="AO1" s="61" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -6763,25 +6754,25 @@
         <v>35</v>
       </c>
       <c r="B1" s="42" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E1" s="51" t="s">
         <v>61</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>35</v>
@@ -6856,7 +6847,7 @@
         <v>57</v>
       </c>
       <c r="AG1" s="58" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -6869,7 +6860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AD1"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AE1" sqref="AE1:XFD1048576"/>
     </sheetView>
@@ -6903,16 +6894,16 @@
         <v>35</v>
       </c>
       <c r="B1" s="59" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C1" s="59" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D1" s="59" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>35</v>
@@ -6987,7 +6978,7 @@
         <v>57</v>
       </c>
       <c r="AD1" s="58" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -7015,16 +7006,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>